<commit_message>
add SSD paper and fix Net.xlsx
</commit_message>
<xml_diff>
--- a/Net.xlsx
+++ b/Net.xlsx
@@ -3,15 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD02B1C7-83A6-C142-8DFD-7B0DCA8E59D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3A4645-E811-E448-BA99-B15E4476324A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="1060" windowWidth="30780" windowHeight="19120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="540" windowWidth="38160" windowHeight="19520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="通用网络" sheetId="4" r:id="rId1"/>
     <sheet name="分类网络" sheetId="1" r:id="rId2"/>
     <sheet name="目标检测" sheetId="2" r:id="rId3"/>
     <sheet name="语义分割" sheetId="3" r:id="rId4"/>
+    <sheet name="模型参数量和计算量计算" sheetId="6" r:id="rId5"/>
+    <sheet name="模型感受野计算" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>论文名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,12 +117,102 @@
     <t>DeepLabv3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>SSD: Single Shot MultiBox Detector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感受野计算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模型参数量计算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卷积层的参数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全链接层参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数量计算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算量计算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="4"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FLOPs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Floating Point Operations)，浮点运算次数，用来衡量算法的时间复杂度</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="4"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FLOPS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Floating Point Operations per Seconds)，单位时间浮点运算次数，用来衡量硬件计算性能。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全链接层的FLOPs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卷积层的FLOPs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +238,49 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="4"/>
@@ -201,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -227,6 +362,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -246,6 +397,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>71887</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>71886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12424299</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3618301</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F83CB47E-0586-8646-AD17-E03AE155743F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6937076" y="299528"/>
+          <a:ext cx="12352412" cy="3546415"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -297,6 +497,3768 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>264160</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2987040" cy="187960"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="文本框 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9CBCAE9-C3CA-D548-B726-6C206AA5BE04}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3556000" y="787400"/>
+              <a:ext cx="2987040" cy="187960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑃𝑎𝑟𝑎𝑚𝑒𝑡𝑒𝑟</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑘</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑤</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>× </m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑘</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>h</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> × </m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐶</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖𝑛</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+1</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> ×  </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐶</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑜𝑢𝑡</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="文本框 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9CBCAE9-C3CA-D548-B726-6C206AA5BE04}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3556000" y="787400"/>
+              <a:ext cx="2987040" cy="187960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑃𝑎𝑟𝑎𝑚𝑒𝑡𝑒𝑟=(𝑘_𝑤  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>× 𝑘_ℎ  × 𝐶_𝑖𝑛+1)  ×  𝐶_𝑜𝑢𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>358702</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>41855</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5345887" cy="191078"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="文本框 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8B3EE13-ABEC-E44C-A661-401406F7D529}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3677635" y="1117122"/>
+              <a:ext cx="5345887" cy="191078"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑘</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑤</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                  <m:r>
+                    <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t> </m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>× </m:t>
+                  </m:r>
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑘</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>h</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                  <m:r>
+                    <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t> × </m:t>
+                  </m:r>
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝐶</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑖𝑛</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示一个卷积核的权重数量</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+                <a:t>,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+                <a:t>+1 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示偏置</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+                <a:t>,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+                <a:t> </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>× </m:t>
+                  </m:r>
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝐶</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑜𝑢𝑡</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示该层有</a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝐶</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑜𝑢𝑡</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>个卷积核 </a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="文本框 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8B3EE13-ABEC-E44C-A661-401406F7D529}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3677635" y="1117122"/>
+              <a:ext cx="5345887" cy="191078"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑘_𝑤  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>× 𝑘_ℎ  × 𝐶_𝑖𝑛</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示一个卷积核的权重数量</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+                <a:t>,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+                <a:t>+1 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示偏置</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+                <a:t>,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>× 𝐶_𝑜𝑢𝑡</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示该层有</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝐶_𝑜𝑢𝑡</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>个卷积核 </a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>220134</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>16934</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2328333" cy="187808"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="文本框 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{241D4900-341A-8141-B19D-2DDA06B36568}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3539067" y="1481667"/>
+              <a:ext cx="2328333" cy="187808"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑃𝑎𝑟𝑎𝑚𝑒𝑡𝑒𝑟</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑁</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖𝑛</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+1</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> ×  </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑁</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑜𝑢𝑡</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="文本框 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{241D4900-341A-8141-B19D-2DDA06B36568}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3539067" y="1481667"/>
+              <a:ext cx="2328333" cy="187808"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑃𝑎𝑟𝑎𝑚𝑒𝑡𝑒𝑟=(𝑁_𝑖𝑛</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>+1)  ×  𝑁_𝑜𝑢𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>327084</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>73848</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4481611" cy="191078"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="文本框 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E297A101-7E0B-CA46-BD8B-721D2D1C8E30}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3646017" y="1733315"/>
+              <a:ext cx="4481611" cy="191078"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑁</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑖𝑛</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示输入的特征向量权重数量</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+                <a:t>, +1 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示偏置</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+                <a:t>,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+                <a:t> </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑁</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑜𝑢𝑡</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                  <m:r>
+                    <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t> </m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示输出的权重数量</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="文本框 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E297A101-7E0B-CA46-BD8B-721D2D1C8E30}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3646017" y="1733315"/>
+              <a:ext cx="4481611" cy="191078"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑁_𝑖𝑛</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示输入的特征向量权重数量</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+                <a:t>, +1 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示偏置</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+                <a:t>,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑁_𝑜𝑢𝑡</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>表示输出的权重数量</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5206999" cy="187808"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="文本框 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6204C06B-973E-454F-B3AE-9D3F9697A030}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3522133" y="3445933"/>
+              <a:ext cx="5206999" cy="187808"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐹𝐿𝑂𝑃𝑠</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="["/>
+                        <m:endChr m:val="]"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="zh-CN" altLang="en-US" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t> </m:t>
+                                </m:r>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝐶</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑖𝑛</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t> </m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>× </m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑘</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑤</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t> × </m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑘</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>h</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:e>
+                        </m:d>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+ </m:t>
+                        </m:r>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="zh-CN" altLang="en-US" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t> </m:t>
+                                </m:r>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝐶</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑖𝑛</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t> </m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>× </m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑘</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑤</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t> × </m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑘</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>h</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t> − 1</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+1</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> ×  </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐶</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑜𝑢𝑡</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> × </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑤</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> × </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>h</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="文本框 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6204C06B-973E-454F-B3AE-9D3F9697A030}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3522133" y="3445933"/>
+              <a:ext cx="5206999" cy="187808"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐹𝐿𝑂𝑃𝑠=[(〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐶〗_𝑖𝑛  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>× 𝑘_𝑤  × 𝑘_ℎ )+ (〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐶〗_𝑖𝑛  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>× 𝑘_𝑤  × 𝑘_ℎ  − 1)+1]  ×  𝐶_𝑜𝑢𝑡  × 𝑤 × ℎ</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>431801</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4293676" cy="174728"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="文本框 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5386B57-BCAC-FA44-B414-64F73B43E8C3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3750734" y="3674533"/>
+              <a:ext cx="4293676" cy="174728"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑤</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="ar-AE" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>和</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>h</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>分别表示卷积核的宽和高</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>, </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>其中</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐶</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>× </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑤</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> × </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>h</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>表示乘法计算量</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="文本框 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5386B57-BCAC-FA44-B414-64F73B43E8C3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3750734" y="3674533"/>
+              <a:ext cx="4293676" cy="174728"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑘_𝑤</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="ar-AE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 和</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ar-AE" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑘〗_ℎ</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 分别表示卷积核的宽和高</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>, </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>其中</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐶〗_𝑖𝑛  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>× 𝑘_𝑤  × 𝑘_ℎ  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>表示乘法计算量</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>364068</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>67732</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7744749" cy="174728"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="文本框 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB0973D7-8663-254C-9FC3-86C09D5BC49B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3683001" y="3886199"/>
+              <a:ext cx="7744749" cy="174728"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐶</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>× </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑤</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> × </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>h</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> −1</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>表示加法计算量</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>, +1</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>表示偏置，</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐶</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑜𝑢𝑡</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> × </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑤</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> × </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>h</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>表示</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑓𝑒𝑎𝑡𝑢𝑟𝑒</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑚𝑎𝑝</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>的所有元素</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>, </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑤</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>, </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>h</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>表示</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑓𝑒𝑎𝑡𝑢𝑟𝑒</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑚𝑎𝑝</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>的宽和高</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="文本框 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB0973D7-8663-254C-9FC3-86C09D5BC49B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3683001" y="3886199"/>
+              <a:ext cx="7744749" cy="174728"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐶〗_𝑖𝑛  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>× 𝑘_𝑤  × 𝑘_ℎ  −1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> 表示加法计算量</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>, +1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>表示偏置，</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐶_𝑜𝑢𝑡  × 𝑤 × ℎ</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> 表示</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓𝑒𝑎𝑡𝑢𝑟𝑒 𝑚𝑎𝑝</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>的所有元素</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>, 𝑤, ℎ </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>表示</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓𝑒𝑎𝑡𝑢𝑟𝑒 𝑚𝑎𝑝</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>的宽和高 </a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1160382" cy="172098"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="文本框 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{042C848A-8F6E-2948-9159-AE922D6F1478}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6201833" y="2624666"/>
+              <a:ext cx="1160382" cy="172098"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <a:fld id="{825F15A7-03F4-43D7-82C5-3E23DA2F108C}" type="mathplaceholder">
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <a:t>在此处键入公式。</a:t>
+                    </a:fld>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="文本框 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{042C848A-8F6E-2948-9159-AE922D6F1478}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6201833" y="2624666"/>
+              <a:ext cx="1160382" cy="172098"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>"在此处键入公式。"</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>105833</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>42332</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2393796" cy="175369"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="文本框 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27A75B7F-CAB5-1646-9B3F-04ADF5831A5F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2595033" y="533399"/>
+              <a:ext cx="2393796" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>神</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                      <m:t>经网络的前向传播</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>: </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑦</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>= </m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑊</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑇</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>× </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑏</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="文本框 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27A75B7F-CAB5-1646-9B3F-04ADF5831A5F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2595033" y="533399"/>
+              <a:ext cx="2393796" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>神"经网络的前向传播</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>": 𝑦= 𝑊^𝑇  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>× 𝑥+𝑏</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>338667</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>16934</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2802468" cy="187808"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="18" name="文本框 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F114D66F-A45E-B143-B36E-825F54C9D135}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3657600" y="4809067"/>
+              <a:ext cx="2802468" cy="187808"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐹𝐿𝑂𝑃𝑠</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="["/>
+                        <m:endChr m:val="]"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼𝑛</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+ </m:t>
+                        </m:r>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐼𝑛</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t> − 1</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+1</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> ×  </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑂𝑢𝑡</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="18" name="文本框 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F114D66F-A45E-B143-B36E-825F54C9D135}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3657600" y="4809067"/>
+              <a:ext cx="2802468" cy="187808"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐹𝐿𝑂𝑃𝑠=[ 𝐼𝑛</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>+ (</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐼𝑛</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> − 1)+1]  ×  𝑂𝑢𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>448735</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2937406" cy="174728"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="19" name="文本框 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B20C543-9A8C-7642-ABD9-8B5B0FF357E7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3767668" y="5071533"/>
+              <a:ext cx="2937406" cy="174728"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐼𝑛</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>和</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑂𝑢𝑡</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>分别表示输入的特征数和输出的特征数</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="19" name="文本框 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B20C543-9A8C-7642-ABD9-8B5B0FF357E7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3767668" y="5071533"/>
+              <a:ext cx="2937406" cy="174728"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐼𝑛</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>和</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑂𝑢𝑡</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>分别表示输入的特征数和输出的特征数</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457202</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3893182" cy="174728"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="20" name="文本框 19">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2069EA1B-11E8-154C-B430-E48FF4032295}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3776135" y="5291667"/>
+              <a:ext cx="3893182" cy="174728"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>其中</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐼𝑛</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>表示乘法运算量</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>, </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐼𝑛</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> −1 </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>表示加法的运算量</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>, +1 </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>表示偏置</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="20" name="文本框 19">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2069EA1B-11E8-154C-B430-E48FF4032295}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3776135" y="5291667"/>
+              <a:ext cx="3893182" cy="174728"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>其中</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐼𝑛</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>表示乘法运算量</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>, 𝐼𝑛 −1 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>表示加法的运算量</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>, +1 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>表示偏置</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1476,19 +5438,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD08288E-7EB8-1F44-898C-CC7A2A6EABCC}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="106" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="62.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="67.6640625" style="9" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="101.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="163.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" customWidth="1"/>
     <col min="7" max="7" width="38.1640625" style="1" customWidth="1"/>
@@ -1526,15 +5488,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="295" customHeight="1">
       <c r="A2" s="2">
         <v>2015</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
+      <c r="B2" s="10" t="s">
+        <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
+      <c r="C2" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1545,8 +5507,8 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1555,9 +5517,15 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1567,8 +5535,8 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1578,8 +5546,8 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1589,8 +5557,8 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1600,8 +5568,8 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1611,8 +5579,8 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1622,8 +5590,8 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1632,8 +5600,8 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1643,8 +5611,8 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1654,8 +5622,8 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1665,8 +5633,8 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1676,8 +5644,8 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1687,8 +5655,8 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1698,8 +5666,8 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1709,8 +5677,8 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1720,8 +5688,8 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1731,8 +5699,8 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1742,8 +5710,8 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1753,8 +5721,8 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1764,8 +5732,8 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1775,8 +5743,8 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1786,8 +5754,8 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1797,8 +5765,8 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -1808,8 +5776,8 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -1819,8 +5787,8 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1830,8 +5798,8 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1841,8 +5809,8 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1852,8 +5820,8 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1863,8 +5831,8 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1874,8 +5842,8 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1885,8 +5853,8 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1896,8 +5864,8 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -1907,8 +5875,8 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1918,8 +5886,8 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1930,6 +5898,8 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1937,7 +5907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282DA812-D402-9D4D-BED3-3746DB64E704}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+    <sheetView zoomScale="109" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2426,4 +6396,122 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C816CAE-D3A4-914C-998B-E1057B5C1882}">
+  <dimension ref="B1:K25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="23">
+      <c r="F1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="5" spans="2:11" ht="16">
+      <c r="B5" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="D7" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="D10" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="16">
+      <c r="B16" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:K1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336D032C-EDE2-7B41-8F7F-DACAA2B7F196}">
+  <dimension ref="I1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="9:16">
+      <c r="I1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+    </row>
+    <row r="2" spans="9:16">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:P2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add two lane paper
</commit_message>
<xml_diff>
--- a/Net.xlsx
+++ b/Net.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358B0C74-0730-4747-A981-A90D6B75C938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388641D2-7453-5E41-9C30-889E25326814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="760" windowWidth="36700" windowHeight="19640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37560" yWindow="20" windowWidth="36700" windowHeight="19640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="通用网络" sheetId="4" r:id="rId1"/>
@@ -15,26 +15,17 @@
     <sheet name="模型参数量和计算量" sheetId="6" r:id="rId5"/>
     <sheet name="模型感受野" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t>论文名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -299,17 +290,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>precision 99.63%
-recall 99.31%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Pytorch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Backbone darknet-53
 Head Yolov3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parking Slot Detection on Around-View Images Using DCNN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type, position, length, and direction of the entrance line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>precision 99.63% @ PS2.0
+recall 99.31% @ PS2.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>precision 99.68% @ PS2.0
+recall 99.41% @ PS2.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>性能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13ms/frame Titan Xp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>512*512</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -441,7 +457,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -482,6 +498,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -688,6 +707,50 @@
         <a:xfrm>
           <a:off x="6949056" y="18235283"/>
           <a:ext cx="8015377" cy="4634373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>71887</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>59905</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10699151</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3836468</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{452353BF-D952-1642-AA05-B0C8CC9BC215}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6937076" y="23003773"/>
+          <a:ext cx="10627264" cy="3776563"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5777,10 +5840,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD08288E-7EB8-1F44-898C-CC7A2A6EABCC}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
@@ -5792,15 +5855,15 @@
     <col min="2" max="2" width="67.6640625" style="9" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="163.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="44.1640625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="8" width="23.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="44.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.1640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="18">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="18">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
@@ -5823,13 +5886,16 @@
         <v>32</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="295" customHeight="1">
+    <row r="2" spans="1:10" ht="295" customHeight="1">
       <c r="A2" s="2">
         <v>2015</v>
       </c>
@@ -5847,14 +5913,15 @@
       <c r="G2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="295" customHeight="1">
+    <row r="3" spans="1:10" ht="295" customHeight="1">
       <c r="A3" s="2">
         <v>2017</v>
       </c>
@@ -5870,12 +5937,13 @@
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="16"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="295" customHeight="1">
+    <row r="4" spans="1:10" ht="295" customHeight="1">
       <c r="A4" s="2">
         <v>2017</v>
       </c>
@@ -5889,12 +5957,13 @@
       <c r="E4" s="2"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="16"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="295" customHeight="1">
+    <row r="5" spans="1:10" ht="295" customHeight="1">
       <c r="A5" s="2">
         <v>2018</v>
       </c>
@@ -5912,12 +5981,13 @@
       <c r="G5" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
+      <c r="H5" s="16"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="216" customHeight="1">
+    <row r="6" spans="1:10" ht="216" customHeight="1">
       <c r="A6" s="2">
         <v>2019</v>
       </c>
@@ -5933,12 +6003,13 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="16">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="16">
       <c r="A7" s="2">
         <v>2015</v>
       </c>
@@ -5954,8 +6025,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="375" customHeight="1">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="375" customHeight="1">
       <c r="A8" s="2">
         <v>2020</v>
       </c>
@@ -5971,27 +6043,41 @@
         <v>53</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="3" t="s">
+    </row>
+    <row r="9" spans="1:10" ht="307" customHeight="1">
+      <c r="A9" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="16">
-      <c r="A9" s="2"/>
-      <c r="B9" s="10"/>
       <c r="C9" s="15"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="16">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="16">
       <c r="A10" s="2"/>
       <c r="B10" s="10"/>
       <c r="C10" s="15"/>
@@ -6001,8 +6087,9 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="16">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="16">
       <c r="A11" s="2"/>
       <c r="B11" s="10"/>
       <c r="C11" s="15"/>
@@ -6012,8 +6099,9 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="16">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="16">
       <c r="A12" s="2"/>
       <c r="B12" s="10"/>
       <c r="C12" s="15"/>
@@ -6023,8 +6111,9 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="16">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="16">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="15"/>
@@ -6032,9 +6121,10 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="16">
+      <c r="H13" s="17"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="16">
       <c r="A14" s="2"/>
       <c r="B14" s="10"/>
       <c r="C14" s="15"/>
@@ -6044,8 +6134,9 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="16">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="16">
       <c r="A15" s="2"/>
       <c r="B15" s="10"/>
       <c r="C15" s="15"/>
@@ -6055,8 +6146,9 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="16">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="16">
       <c r="A16" s="2"/>
       <c r="B16" s="10"/>
       <c r="C16" s="15"/>
@@ -6066,8 +6158,9 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="16">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" ht="16">
       <c r="A17" s="2"/>
       <c r="B17" s="10"/>
       <c r="C17" s="15"/>
@@ -6077,8 +6170,9 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="16">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" ht="16">
       <c r="A18" s="2"/>
       <c r="B18" s="10"/>
       <c r="C18" s="15"/>
@@ -6088,8 +6182,9 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" ht="16">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" ht="16">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="15"/>
@@ -6099,8 +6194,9 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="16">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" ht="16">
       <c r="A20" s="2"/>
       <c r="B20" s="10"/>
       <c r="C20" s="15"/>
@@ -6110,8 +6206,9 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" ht="16">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" ht="16">
       <c r="A21" s="2"/>
       <c r="B21" s="10"/>
       <c r="C21" s="15"/>
@@ -6121,8 +6218,9 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" ht="16">
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" ht="16">
       <c r="A22" s="2"/>
       <c r="B22" s="10"/>
       <c r="C22" s="15"/>
@@ -6132,8 +6230,9 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" ht="16">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" ht="16">
       <c r="A23" s="2"/>
       <c r="B23" s="10"/>
       <c r="C23" s="15"/>
@@ -6143,8 +6242,9 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" ht="16">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" ht="16">
       <c r="A24" s="2"/>
       <c r="B24" s="10"/>
       <c r="C24" s="15"/>
@@ -6154,8 +6254,9 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" ht="16">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" ht="16">
       <c r="A25" s="2"/>
       <c r="B25" s="10"/>
       <c r="C25" s="15"/>
@@ -6165,8 +6266,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="16">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" ht="16">
       <c r="A26" s="2"/>
       <c r="B26" s="10"/>
       <c r="C26" s="15"/>
@@ -6176,8 +6278,9 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" ht="16">
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" ht="16">
       <c r="A27" s="2"/>
       <c r="B27" s="10"/>
       <c r="C27" s="15"/>
@@ -6187,8 +6290,9 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" ht="16">
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" ht="16">
       <c r="A28" s="2"/>
       <c r="B28" s="10"/>
       <c r="C28" s="15"/>
@@ -6198,8 +6302,9 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" ht="16">
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" ht="16">
       <c r="A29" s="2"/>
       <c r="B29" s="10"/>
       <c r="C29" s="15"/>
@@ -6209,8 +6314,9 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="16">
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" ht="16">
       <c r="A30" s="2"/>
       <c r="B30" s="10"/>
       <c r="C30" s="15"/>
@@ -6220,8 +6326,9 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="16">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" ht="16">
       <c r="A31" s="2"/>
       <c r="B31" s="10"/>
       <c r="C31" s="15"/>
@@ -6231,8 +6338,9 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" ht="16">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" ht="16">
       <c r="A32" s="2"/>
       <c r="B32" s="10"/>
       <c r="C32" s="15"/>
@@ -6242,8 +6350,9 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" ht="16">
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" ht="16">
       <c r="A33" s="2"/>
       <c r="B33" s="10"/>
       <c r="C33" s="15"/>
@@ -6253,8 +6362,9 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" ht="16">
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" ht="16">
       <c r="A34" s="2"/>
       <c r="B34" s="10"/>
       <c r="C34" s="15"/>
@@ -6264,8 +6374,9 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" ht="16">
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" ht="16">
       <c r="A35" s="2"/>
       <c r="B35" s="10"/>
       <c r="C35" s="15"/>
@@ -6275,8 +6386,9 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" ht="16">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" ht="16">
       <c r="A36" s="2"/>
       <c r="B36" s="10"/>
       <c r="C36" s="15"/>
@@ -6286,8 +6398,9 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" ht="16">
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" ht="16">
       <c r="A37" s="2"/>
       <c r="B37" s="10"/>
       <c r="C37" s="15"/>
@@ -6297,8 +6410,9 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" ht="16">
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" ht="16">
       <c r="A38" s="2"/>
       <c r="B38" s="10"/>
       <c r="C38" s="15"/>
@@ -6308,8 +6422,9 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" ht="16">
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" ht="16">
       <c r="A39" s="2"/>
       <c r="B39" s="10"/>
       <c r="C39" s="15"/>
@@ -6319,8 +6434,9 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" ht="16">
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" ht="16">
       <c r="A40" s="2"/>
       <c r="B40" s="10"/>
       <c r="C40" s="15"/>
@@ -6330,6 +6446,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6848,14 +6965,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="23">
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="5" spans="2:11" ht="16">
       <c r="B5" s="14" t="s">
@@ -6922,26 +7039,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:16">
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" spans="4:16">
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
     </row>
     <row r="7" spans="4:16">
       <c r="D7"/>

</xml_diff>

<commit_message>
add Deformable ConvNets Paper
</commit_message>
<xml_diff>
--- a/Net.xlsx
+++ b/Net.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42B9058-4A64-D041-A40B-2AD3F1D985D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0077A93-BC81-234B-A9D8-8C04AFAF45F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="36700" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="36700" windowHeight="19640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="通用网络" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="70">
   <si>
     <t>论文名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -349,6 +349,19 @@
     <t>ViT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Objects as Points</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anchor-Free</t>
+  </si>
+  <si>
+    <t>28.1% AP at 142 FPS@MS COCO
+37.4% AP at 52 FPS@MS COCO
+45.1% AP with multi-scale testing at 1.4 FPS@MS COCO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -459,7 +472,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -482,12 +495,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -559,14 +598,20 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -772,6 +817,56 @@
         <a:xfrm>
           <a:off x="6961038" y="11501887"/>
           <a:ext cx="6889151" cy="3595028"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>155754</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>83867</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8893471</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2647830</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBBF509C-14DD-8943-9AFA-39F8F1E715BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7020943" y="18055565"/>
+          <a:ext cx="8737717" cy="2563963"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5089,7 +5184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC0A13B-1CE3-F041-82C4-0947D02261D3}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+    <sheetView zoomScale="156" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5153,7 +5248,7 @@
       <c r="A2" s="18">
         <v>2021</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -6242,13 +6337,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD08288E-7EB8-1F44-898C-CC7A2A6EABCC}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView zoomScale="106" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O28" sqref="O28"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6428,30 +6523,40 @@
       </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="16">
+    <row r="7" spans="1:12" ht="216" customHeight="1">
       <c r="A7" s="2">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="I7" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="31"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="16">
-      <c r="A8" s="2"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="15"/>
+      <c r="A8" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -6500,7 +6605,8 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="17"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="16">
@@ -6513,8 +6619,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="J12" s="17"/>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="16">
@@ -6909,7 +7014,24 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
+    <row r="41" spans="1:12" ht="16">
+      <c r="A41" s="2"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I7:J7"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8741,14 +8863,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="23">
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="5" spans="2:11" ht="16">
       <c r="B5" s="14" t="s">
@@ -8815,26 +8937,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:16">
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="4:16">
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
     </row>
     <row r="7" spans="4:16">
       <c r="D7"/>

</xml_diff>